<commit_message>
removed faculty accessing error
</commit_message>
<xml_diff>
--- a/chatbotdb.xlsx
+++ b/chatbotdb.xlsx
@@ -376,7 +376,7 @@
     <t xml:space="preserve">Ubiquitous Computing Group</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
+    <t xml:space="preserve">multiple</t>
   </si>
   <si>
     <t xml:space="preserve">http://gvu.gatech.edu/research/labs/ubiquitous-computing-group</t>
@@ -790,17 +790,17 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,7 +1438,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,7 +1634,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +1879,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated DB to include multiple fields
</commit_message>
<xml_diff>
--- a/chatbotdb.xlsx
+++ b/chatbotdb.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="211">
   <si>
     <t xml:space="preserve">lab_name</t>
   </si>
@@ -58,518 +58,532 @@
     <t xml:space="preserve">This lab explores the emerging area of animal-computer interaction focusing on interfaces for inter-species communication and on the design and evaluation of interactive technology for users of multiple species.</t>
   </si>
   <si>
+    <t xml:space="preserve">interactive technology,AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augmented Environments Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blair MacIntyre, Jay Bolter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://ael.gatech.edu/lab/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab activities focus on understanding how to build interactive computing environments that directly augment a user's senses with computer-generated material. Researchers are interested in augmenting the user's perception, and place particular emphasis on the interaction between the users and their environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">augmented reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BrainLab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melody Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://brainlab.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Brain Lab explores innovative ways of accomplishing human-computer interaction through biometric inputs. Biometric interfaces identify and measure small changes in a person's behavior or physiological responses to certain stimuli. The work has potential in many areas, especially for providing individuals with disabilities a means of personal "hands-off" control of computers and other devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biometrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comp.social lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eric Gilbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://comp.social.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The comp.social lab focuses on the design and analysis of social media. According to their website, lab researchers "like puppies, mixed methods, and new students (particularly M.S.)."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">social media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computational Enterprise Science Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahul Basole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gvu.gatech.edu/research/labs/computational-enterprise-science-lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Computational Enterprise Science Lab focuses on the design, analysis, and management of complex enterprise systems (e.g. organizations, supply chains, business ecosystems) using information visualization, modeling/simulation, and system science approaches.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">information visualization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computational Linguistics Laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacob Eisenstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gtnlp.wordpress.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This lab works on machine learning approaches to understanding human language and is especially interested in non-standard language, discourse, computational social science, and statistical machine learning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natural language,ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computational Perception Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron Bobick, Tucker Balch, Henrik Christensen, Frank Dellaert, Irfan Essa , Jim Rehg, Thad Starner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/cpl/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Computational Perception Laboratory (CPL) was established to explore and develop the next generation of intelligent machines, interfaces, and environments for modeling, perceiving, recognizing, and interacting with humans and for all forms of behavior analysis from data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer vision,ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contextual Computing Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thad Starner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://research.cc.gatech.edu/ccg/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Contextual Computing Group develops applications and interfaces for the computer to be aware of what the user is doing and to assist the user as appropriate. Several current projects at the research stage are envisioned to work together to assist a user in routine tasks such as automatically scheduling an appointment, re-directing an urgent phone call appropriately based on the user's schedule and current activity, and recognizing that the user is engaged in conversation and would prefer to take the phone call later.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contextual computing,AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contextualized Support for Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark Guzdial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://home.cc.gatech.edu/csl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Led by Mark Guzdial, the Contextualized Support for Learning (CSL) lab has as its aim the creation of "collaborative Dynabooks." We are a team of faculty, graduate, and undergraduate students who design and implement innovative technology with the goal of improving learning, then empirically explore the benefits and usefulness of the technology with real users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Culture and Technology Lab (CAT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betsy DiSalvo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://catlab.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CAT Lab studies how culture impacts the use and production of technology with a focus on learning applications, computer science education and the design of new technologies, with culture as a point of convergence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">education,culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design &amp; Intelligence Laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashok Goel, Keith McGreggor, Spencer Rugaber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://dilab.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Design &amp; Intelligence Laboratory conducts research into human-centered artificial intelligence and computational cognitive science, with a focus on computational creativity. Current projects explore analogical reasoning in biologically inspired design, visual reasoning on intelligence tests, meta-reasoning in game-playing software agents, and learning about ecological and biological systems in science education.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronic Learning Communities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amy Bruckman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/elc/index.shtml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The concept that people learn best when they are making something personally meaningful—also known as constructionism—is the lab's guiding philosophy. Computer networks have the potential to facilitate community-supported constructionist learning. The Electronic Learning Communities Lab examines ways communities of learners can motivate and support one another's learning experiences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entertainment Intelligence Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark Riedl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://research.cc.gatech.edu/eilab/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Entertainment Intelligence Lab focuses on computational approaches to creating engaging and entertaining experiences. Some of the problem domains they work on include computer games, storytelling, interactive digital worlds, adaptive media, and procedural content generation. They expressly focus on computationally "hard" problems that require automation, just-in-time generation, and scalability of personalized experiences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everyday Computing Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beth Mynatt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://research.cc.gatech.edu/ecl/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We introduce a new area of interaction research, everyday computing, by focusing on scaling ubiquitous computing with respect to time. Our motivations for everyday computing stem from the desire to support the informal, unstructured activities typical of our everyday lives. Our goal is to understand the transformation of everyday life as computing is ubiquitously integrated into informal, daily activities and routines.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ubiquitous computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphics Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greg Turk, Karen Liu, Jarek Rossignac, Irfan Essa, Jim Rehg, Blair MacIntyre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/graphics/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Graphics Lab is dedicated to research in all aspects of computer graphics, including animation, modeling, rendering, image and video manipulation, and augmented reality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Interfaces Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Stasko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/gvu/ii/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the Information Interfaces Lab, computing technologies are developed that help people take advantage of information to enrich their lives. The lab group develops ways to help people understand information via user interface design, information visualization, peripheral awareness techniques, and embodied agents. The goal is to help people make better judgments by learning from all the information available to them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratory for Interactive Artificial Intelligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charles Isbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/~isbell/iai/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our fundamental research goal is to understand how to build autonomous agents that live and interact with large numbers of other intelligent agents, some of whom may be human. Progress towards this goal means that we can build artificial systems that work with humans to accomplish tasks more effectively; can be more robust to changes in environment, relationships, and goals; and can better co-exist with humans as long-lived partners.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI,ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarek Rossignac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/~jarek/magic/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our research focuses on the design, representation, simplification, compression, analysis, and visualization of highly complex 3D shapes, structures, and animations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Robot Laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ron Arkin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/ai/robot-lab/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The role of the Mobile Robot Laboratory is to discover and develop fundamental scientific principles and practices that are applicable to intelligent mobile-robot systems. In addition, the laboratory facilitates technology transfer of its research results to yield solutions for a range of applications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">robotics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIXI Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keith Edwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/pixi/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PIXI Lab is a group of researchers at the GVU Center at Georgia Tech who are exploring the boundaries between interaction and infrastructure. We take a human-centered approach to our research, by understanding the needs and practices of people through empirical methods, designing compelling user experiences that fit that context, and then building the underlying systems and networking infrastructure necessary to realize that user experience. We are dedicated to creating technology that is not simply usable but also useful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Dynamics and Well Being Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munmun De Choudhury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gvu.gatech.edu/research/labs/social-dynamics-and-wellbeing-lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Social Dynamics and Wellbeing Lab studies, mines and analyzes social media to derive insights into improving our health and well-being.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">social networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socially Intelligent Machines Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea Thomaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/social-machines/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The vision of our research is to enable robots to function in dynamic human environments by allowing them to flexibly adapt their skill set via learning interactions with end-users. We call this Socially Guided Machine Learning (SG-ML), exploring the ways in which machine learning agents can exploit principles of human social learning. To date, our work in SG-ML has focused on two research thrusts: (1) interactive machine learning, and (2) natural interaction patterns for HRI. Here you will find recent examples of projects in each of these two thrusts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technologies and International Development Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Best</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://tid.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The lab's research focuses on information and communication technologies for social, economic, and political development. In particular the lab studies mobile phones, the Internet, and Internet-enabled services and their design, impact, and importance within low-income countries of Africa and Asia. The lab researches engineering, public policy, HCI/usability, and sustainability issues as methods to assess and evaluate social, economic, and political development outcomes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubiquitous Computing Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gvu.gatech.edu/research/labs/ubiquitous-computing-group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are interested in ubiquitous computing (ubicomp) and the research issues involved in building and evaluating ubicomp applications and services that impact our lives. Much of our work is situated in settings of everyday activity, such as the classroom, the office, and the home. Our research focuses on several topics including, automated capture and access to live experiences, context-aware computing, applications and services in the home, natural interaction, software architecture, technology policy, security and privacy issues, and technology for individuals with special needs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">App Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt Sanders, Russ Clark, Keith Edwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://gtjourney.gatech.edu/rnoc-lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are encouraged to take advantage of the App Lab regardless of their major. Open to any GT student interested in using its resources. Clubs and classes are encouraged to take advantage of the resources without disrupting individuals working there as well. A “hackerspace” devoted to the creation of mobile applications and technologies across a range of platforms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobile applications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAM Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brian Magerko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.gvu.gatech.edu/research/labs/adam-lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Adaptive Media Lab explores how to create digital media experiences that tailor themselves to individual users. These adaptations may occur for dramatic purposes (e.g. interactive narrative), educational purposes (e.g. serious games), and / or purely for entertainment. This research involves work in design, artificial intelligence, and human computer interaction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work 2 Play Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rebecca E. Grinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/~beki/wpl/Work2Play.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the last decade, computing has left the office and entered people's domestic and recreational lives. Consequently, computing affects our lives, shaping not just how we work, but also how we play. Moreover, computing potentially allows individuals to blur the boundaries by letting us conduct domestic routines while in the office, or working from a cafe in an urban center. Researchers in the Work 2 Play Lab are interested in using a variety of empirical techniques to advance the state of the knowledge in how computing affects our lives from work to play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonification Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruce N. Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://sonify.psych.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonification Lab focuses on the development and evaluation of auditory and multimodal interfaces, and the cognitive, psychophysical and practical aspects of auditory displays, paying particular attention to sonification. Special consideration is paid to Human Factors in the display of information in "complex task environments," such as the human-computer interfaces in cockpits, nuclear powerplants, in-vehicle infotainment displays, and in the space program.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparch Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Conte, Hadi Esmaeilzadeh, Hyesoon Kim, Santosh Pande, Milos Prvulovic, Kishore Ramachandran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School of Computer Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://comparch.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Computer Architecture (comparch) Lab conducts research on all aspects of future microprocessor technology including performance, power, multi-threading, chip-multiprocessing, security, programmability, reliability, interaction with compilers and software, and the impact of future technologies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributed Data Intensive Systems Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ling Liu, Calton Pu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/projects/disl/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DiSL offers research expertise in distributed and Internet computing systems and distributed data intensive systems. Most of the research projects conducted in DiSL have strong emphasis on systems issues such as scalability, reliability, security, availability and efficiency, and data management issues such as data storage, data mining and data analysis. We are interested in theories and techniques that not only make the distributed systems scalable and efficient but also reliable and secure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distributed computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embedded Pervasive Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kishore Ramachandran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://wiki.cc.gatech.edu/epl/index.php/Main_Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research in the Embedded Pervasive Lab (EPL) covers a range of topics including distributed programming idioms, networked embedded sensors, P2P video streaming, middleware for efficient large-scale stream processing, opportunistic networking, virtualization technologies, and smart storages incorporating Flash-based SSDs. EPL is producing systems for a world where machines, devices and networking technologies work in concert to help individuals use them with as little instruction as possible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">embedded computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korvo Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karsten Schwan, Greg Eisenhauer, Ada Gavriloska, Matthew Wolf, Jeff Young</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://korvo.gatech.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Korvo research group of researchers focuses on pushing the boundaries of computer systems research. We take an experimental approach to computer systems, working heavily with industry and governmental stakeholders with real-world problems as motivation for our efforts to refine and fundamentally restructure the way operating systems work. Our interests cover the areas of Cloud Computing, High Performance Computing, and Internet of Things, with particular focus on building systems that can deal with tight orchestration of large streams of data, wherever that data source may come from.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cloud computing, IOT, high performance computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrustAble Programming Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William Harris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.cc.gatech.edu/~wharris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In today’s computing environments, writing a mostly-functioning program is hard enough, and writing a completely secure program is often practically impossible. The Trustable Programming (TAP) Group extends and applies techniques from program analysis and synthesis to make these problems tractable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">information security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Networks Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostafa Ammar, Constantine Dovrolis, Jim Xu, Ellen Zegura, Russ Clark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.scs.gatech.edu/content/networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The networks group aims to understand and advance the theory and practice of networks, whether they be mobile, wireless, Internet, campus, home, physical, virtual, human-constructed or naturally occurring. They combine modeling with measurement and experimentation to connect insights to novel approaches to solving problems. Areas of expertise include network algorithmics, multicast, multimedia, disruption-tolerant networking, mobile computing, network operations, Internet economics, and network science.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theory Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lance Fortnow, Zvi Galil, Dick Lipton, Milena Mihail, Chris Peikert, Richard Peng, Dana Randall, Prasad Tetali, Vijay Vazirani, Santosh Vempala, H. Venkateswaran, Eric Vigoda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cc.gatech.edu/theory/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The theory group has expertise spanning foundations and applications of algorithms and computational complexity theory, including combinatorial optimization, approximation algorithms, randomized algorithms, stochastic processes, spectral methods, algorithmic game theory, high-dimensional geometry, network models, and cryptography. The theory group also constitutes some of the core faculty of both the College of Computing’s Algorithms &amp; Randomness Center (ARC) and Georgia Tech’s Ph.D. program in Algorithms, Combinatorics and Optimization (ACO).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">algorithms, theory</t>
+  </si>
+  <si>
     <t xml:space="preserve">interactive technology</t>
   </si>
   <si>
-    <t xml:space="preserve">Augmented Environments Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blair MacIntyre, Jay Bolter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ael.gatech.edu/lab/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lab activities focus on understanding how to build interactive computing environments that directly augment a user's senses with computer-generated material. Researchers are interested in augmenting the user's perception, and place particular emphasis on the interaction between the users and their environment.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">augmented reality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BrainLab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melody Jackson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://brainlab.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Brain Lab explores innovative ways of accomplishing human-computer interaction through biometric inputs. Biometric interfaces identify and measure small changes in a person's behavior or physiological responses to certain stimuli. The work has potential in many areas, especially for providing individuals with disabilities a means of personal "hands-off" control of computers and other devices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biometrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comp.social lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eric Gilbert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://comp.social.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The comp.social lab focuses on the design and analysis of social media. According to their website, lab researchers "like puppies, mixed methods, and new students (particularly M.S.)."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">social media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computational Enterprise Science Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rahul Basole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://gvu.gatech.edu/research/labs/computational-enterprise-science-lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Computational Enterprise Science Lab focuses on the design, analysis, and management of complex enterprise systems (e.g. organizations, supply chains, business ecosystems) using information visualization, modeling/simulation, and system science approaches.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">information visualization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computational Linguistics Laboratory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacob Eisenstein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://gtnlp.wordpress.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This lab works on machine learning approaches to understanding human language and is especially interested in non-standard language, discourse, computational social science, and statistical machine learning.</t>
+    <t xml:space="preserve">human-computer interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infoviz</t>
   </si>
   <si>
     <t xml:space="preserve">natural language</t>
   </si>
   <si>
-    <t xml:space="preserve">Computational Perception Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aaron Bobick, Tucker Balch, Henrik Christensen, Frank Dellaert, Irfan Essa , Jim Rehg, Thad Starner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/cpl/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Computational Perception Laboratory (CPL) was established to explore and develop the next generation of intelligent machines, interfaces, and environments for modeling, perceiving, recognizing, and interacting with humans and for all forms of behavior analysis from data.</t>
+    <t xml:space="preserve">natural language processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP</t>
   </si>
   <si>
     <t xml:space="preserve">computer vision</t>
   </si>
   <si>
-    <t xml:space="preserve">Contextual Computing Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thad Starner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://research.cc.gatech.edu/ccg/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Contextual Computing Group develops applications and interfaces for the computer to be aware of what the user is doing and to assist the user as appropriate. Several current projects at the research stage are envisioned to work together to assist a user in routine tasks such as automatically scheduling an appointment, re-directing an urgent phone call appropriately based on the user's schedule and current activity, and recognizing that the user is engaged in conversation and would prefer to take the phone call later.</t>
+    <t xml:space="preserve">computational perception</t>
   </si>
   <si>
     <t xml:space="preserve">contextual computing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contextualized Support for Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mark Guzdial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://home.cc.gatech.edu/csl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Led by Mark Guzdial, the Contextualized Support for Learning (CSL) lab has as its aim the creation of "collaborative Dynabooks." We are a team of faculty, graduate, and undergraduate students who design and implement innovative technology with the goal of improving learning, then empirically explore the benefits and usefulness of the technology with real users.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Culture and Technology Lab (CAT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betsy DiSalvo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://catlab.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The CAT Lab studies how culture impacts the use and production of technology with a focus on learning applications, computer science education and the design of new technologies, with culture as a point of convergence.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design &amp; Intelligence Laboratory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ashok Goel, Keith McGreggor, Spencer Rugaber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://dilab.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Design &amp; Intelligence Laboratory conducts research into human-centered artificial intelligence and computational cognitive science, with a focus on computational creativity. Current projects explore analogical reasoning in biologically inspired design, visual reasoning on intelligence tests, meta-reasoning in game-playing software agents, and learning about ecological and biological systems in science education.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronic Learning Communities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amy Bruckman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/elc/index.shtml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The concept that people learn best when they are making something personally meaningful—also known as constructionism—is the lab's guiding philosophy. Computer networks have the potential to facilitate community-supported constructionist learning. The Electronic Learning Communities Lab examines ways communities of learners can motivate and support one another's learning experiences.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entertainment Intelligence Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mark Riedl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://research.cc.gatech.edu/eilab/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Entertainment Intelligence Lab focuses on computational approaches to creating engaging and entertaining experiences. Some of the problem domains they work on include computer games, storytelling, interactive digital worlds, adaptive media, and procedural content generation. They expressly focus on computationally "hard" problems that require automation, just-in-time generation, and scalability of personalized experiences.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Everyday Computing Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beth Mynatt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://research.cc.gatech.edu/ecl/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We introduce a new area of interaction research, everyday computing, by focusing on scaling ubiquitous computing with respect to time. Our motivations for everyday computing stem from the desire to support the informal, unstructured activities typical of our everyday lives. Our goal is to understand the transformation of everyday life as computing is ubiquitously integrated into informal, daily activities and routines.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ubiquitous computing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graphics Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greg Turk, Karen Liu, Jarek Rossignac, Irfan Essa, Jim Rehg, Blair MacIntyre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/graphics/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Graphics Lab is dedicated to research in all aspects of computer graphics, including animation, modeling, rendering, image and video manipulation, and augmented reality.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">graphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information Interfaces Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Stasko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/gvu/ii/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At the Information Interfaces Lab, computing technologies are developed that help people take advantage of information to enrich their lives. The lab group develops ways to help people understand information via user interface design, information visualization, peripheral awareness techniques, and embodied agents. The goal is to help people make better judgments by learning from all the information available to them.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laboratory for Interactive Artificial Intelligence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charles Isbell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/~isbell/iai/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Our fundamental research goal is to understand how to build autonomous agents that live and interact with large numbers of other intelligent agents, some of whom may be human. Progress towards this goal means that we can build artificial systems that work with humans to accomplish tasks more effectively; can be more robust to changes in environment, relationships, and goals; and can better co-exist with humans as long-lived partners.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magic Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jarek Rossignac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/~jarek/magic/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Our research focuses on the design, representation, simplification, compression, analysis, and visualization of highly complex 3D shapes, structures, and animations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile Robot Laboratory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ron Arkin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/ai/robot-lab/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The role of the Mobile Robot Laboratory is to discover and develop fundamental scientific principles and practices that are applicable to intelligent mobile-robot systems. In addition, the laboratory facilitates technology transfer of its research results to yield solutions for a range of applications.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">robotics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIXI Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keith Edwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/pixi/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The PIXI Lab is a group of researchers at the GVU Center at Georgia Tech who are exploring the boundaries between interaction and infrastructure. We take a human-centered approach to our research, by understanding the needs and practices of people through empirical methods, designing compelling user experiences that fit that context, and then building the underlying systems and networking infrastructure necessary to realize that user experience. We are dedicated to creating technology that is not simply usable but also useful.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Dynamics and Well Being Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munmun De Choudhury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://gvu.gatech.edu/research/labs/social-dynamics-and-wellbeing-lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Social Dynamics and Wellbeing Lab studies, mines and analyzes social media to derive insights into improving our health and well-being.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">social networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socially Intelligent Machines Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea Thomaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/social-machines/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The vision of our research is to enable robots to function in dynamic human environments by allowing them to flexibly adapt their skill set via learning interactions with end-users. We call this Socially Guided Machine Learning (SG-ML), exploring the ways in which machine learning agents can exploit principles of human social learning. To date, our work in SG-ML has focused on two research thrusts: (1) interactive machine learning, and (2) natural interaction patterns for HRI. Here you will find recent examples of projects in each of these two thrusts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technologies and International Development Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Michael Best</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://tid.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The lab's research focuses on information and communication technologies for social, economic, and political development. In particular the lab studies mobile phones, the Internet, and Internet-enabled services and their design, impact, and importance within low-income countries of Africa and Asia. The lab researches engineering, public policy, HCI/usability, and sustainability issues as methods to assess and evaluate social, economic, and political development outcomes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ubiquitous Computing Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multiple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://gvu.gatech.edu/research/labs/ubiquitous-computing-group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We are interested in ubiquitous computing (ubicomp) and the research issues involved in building and evaluating ubicomp applications and services that impact our lives. Much of our work is situated in settings of everyday activity, such as the classroom, the office, and the home. Our research focuses on several topics including, automated capture and access to live experiences, context-aware computing, applications and services in the home, natural interaction, software architecture, technology policy, security and privacy issues, and technology for individuals with special needs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">App Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matt Sanders, Russ Clark, Keith Edwards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://gtjourney.gatech.edu/rnoc-lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are encouraged to take advantage of the App Lab regardless of their major. Open to any GT student interested in using its resources. Clubs and classes are encouraged to take advantage of the resources without disrupting individuals working there as well. A “hackerspace” devoted to the creation of mobile applications and technologies across a range of platforms.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobile applications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADAM Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brian Magerko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.gvu.gatech.edu/research/labs/adam-lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Adaptive Media Lab explores how to create digital media experiences that tailor themselves to individual users. These adaptations may occur for dramatic purposes (e.g. interactive narrative), educational purposes (e.g. serious games), and / or purely for entertainment. This research involves work in design, artificial intelligence, and human computer interaction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work 2 Play Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rebecca E. Grinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/~beki/wpl/Work2Play.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the last decade, computing has left the office and entered people's domestic and recreational lives. Consequently, computing affects our lives, shaping not just how we work, but also how we play. Moreover, computing potentially allows individuals to blur the boundaries by letting us conduct domestic routines while in the office, or working from a cafe in an urban center. Researchers in the Work 2 Play Lab are interested in using a variety of empirical techniques to advance the state of the knowledge in how computing affects our lives from work to play.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ubiquitous computing
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonification Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bruce N. Walker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://sonify.psych.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonification Lab focuses on the development and evaluation of auditory and multimodal interfaces, and the cognitive, psychophysical and practical aspects of auditory displays, paying particular attention to sonification. Special consideration is paid to Human Factors in the display of information in "complex task environments," such as the human-computer interfaces in cockpits, nuclear powerplants, in-vehicle infotainment displays, and in the space program.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparch Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom Conte, Hadi Esmaeilzadeh, Hyesoon Kim, Santosh Pande, Milos Prvulovic, Kishore Ramachandran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School of Computer Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://comparch.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Computer Architecture (comparch) Lab conducts research on all aspects of future microprocessor technology including performance, power, multi-threading, chip-multiprocessing, security, programmability, reliability, interaction with compilers and software, and the impact of future technologies.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">computer architecture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distributed Data Intensive Systems Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ling Liu, Calton Pu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/projects/disl/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DiSL offers research expertise in distributed and Internet computing systems and distributed data intensive systems. Most of the research projects conducted in DiSL have strong emphasis on systems issues such as scalability, reliability, security, availability and efficiency, and data management issues such as data storage, data mining and data analysis. We are interested in theories and techniques that not only make the distributed systems scalable and efficient but also reliable and secure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distributed computing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Embedded Pervasive Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kishore Ramachandran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://wiki.cc.gatech.edu/epl/index.php/Main_Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research in the Embedded Pervasive Lab (EPL) covers a range of topics including distributed programming idioms, networked embedded sensors, P2P video streaming, middleware for efficient large-scale stream processing, opportunistic networking, virtualization technologies, and smart storages incorporating Flash-based SSDs. EPL is producing systems for a world where machines, devices and networking technologies work in concert to help individuals use them with as little instruction as possible.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">embedded computing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korvo Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karsten Schwan, Greg Eisenhauer, Ada Gavriloska, Matthew Wolf, Jeff Young</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://korvo.gatech.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Korvo research group of researchers focuses on pushing the boundaries of computer systems research. We take an experimental approach to computer systems, working heavily with industry and governmental stakeholders with real-world problems as motivation for our efforts to refine and fundamentally restructure the way operating systems work. Our interests cover the areas of Cloud Computing, High Performance Computing, and Internet of Things, with particular focus on building systems that can deal with tight orchestration of large streams of data, wherever that data source may come from.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cloud computing, IOT, high performance computing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrustAble Programming Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William Harris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.cc.gatech.edu/~wharris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In today’s computing environments, writing a mostly-functioning program is hard enough, and writing a completely secure program is often practically impossible. The Trustable Programming (TAP) Group extends and applies techniques from program analysis and synthesis to make these problems tractable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">information security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Networks Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mostafa Ammar, Constantine Dovrolis, Jim Xu, Ellen Zegura, Russ Clark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.scs.gatech.edu/content/networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The networks group aims to understand and advance the theory and practice of networks, whether they be mobile, wireless, Internet, campus, home, physical, virtual, human-constructed or naturally occurring. They combine modeling with measurement and experimentation to connect insights to novel approaches to solving problems. Areas of expertise include network algorithmics, multicast, multimedia, disruption-tolerant networking, mobile computing, network operations, Internet economics, and network science.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theory Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lance Fortnow, Zvi Galil, Dick Lipton, Milena Mihail, Chris Peikert, Richard Peng, Dana Randall, Prasad Tetali, Vijay Vazirani, Santosh Vempala, H. Venkateswaran, Eric Vigoda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cc.gatech.edu/theory/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The theory group has expertise spanning foundations and applications of algorithms and computational complexity theory, including combinatorial optimization, approximation algorithms, randomized algorithms, stochastic processes, spectral methods, algorithmic game theory, high-dimensional geometry, network models, and cryptography. The theory group also constitutes some of the core faculty of both the College of Computing’s Algorithms &amp; Randomness Center (ARC) and Georgia Tech’s Ph.D. program in Algorithms, Combinatorics and Optimization (ACO).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">algorithms, theory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">human-computer interaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infoviz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natural language processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">computational perception</t>
   </si>
   <si>
     <t xml:space="preserve">user context</t>
@@ -789,18 +803,18 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,44 +1035,44 @@
         <v>55</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>51</v>
@@ -1066,79 +1080,79 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>31</v>
@@ -1146,242 +1160,242 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>134</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1438,7 +1452,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,142 +1477,142 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1634,18 +1648,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1677,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,34 +1685,34 @@
         <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>181</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>184</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>186</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,151 +1722,151 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1893,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,92 +1948,92 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>